<commit_message>
update template analysis for plate reader growth curves
</commit_message>
<xml_diff>
--- a/templates/growth_plate_reader/DATE_plate_layout.xlsx
+++ b/templates/growth_plate_reader/DATE_plate_layout.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/razo/Documents/PhD/evo_mwc/templates/growth_plate_reader/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrazomej/git/fit_seq/templates/growth_plate_reader/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68B72D6-F538-BB4D-A923-C1F42FF8C0C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strain" sheetId="1" r:id="rId1"/>
     <sheet name="well" sheetId="5" r:id="rId2"/>
     <sheet name="media" sheetId="2" r:id="rId3"/>
     <sheet name="pos_selection" sheetId="3" r:id="rId4"/>
-    <sheet name="neg_selection" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="99">
   <si>
     <t>B10</t>
   </si>
@@ -327,17 +327,23 @@
     <t>x_units_compound</t>
   </si>
   <si>
-    <t>op_rep_selection</t>
+    <t>prom_T_marker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -374,6 +380,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -641,14 +650,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -955,12 +969,13 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1279,7 +1294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1601,10 +1616,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
@@ -1920,323 +1935,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I3" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" t="s">
-        <v>97</v>
-      </c>
-      <c r="L3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J4" t="s">
-        <v>97</v>
-      </c>
-      <c r="K4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J5" t="s">
-        <v>97</v>
-      </c>
-      <c r="K5" t="s">
-        <v>97</v>
-      </c>
-      <c r="L5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" t="s">
-        <v>97</v>
-      </c>
-      <c r="I6" t="s">
-        <v>97</v>
-      </c>
-      <c r="J6" t="s">
-        <v>97</v>
-      </c>
-      <c r="K6" t="s">
-        <v>97</v>
-      </c>
-      <c r="L6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" t="s">
-        <v>97</v>
-      </c>
-      <c r="H7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I7" t="s">
-        <v>97</v>
-      </c>
-      <c r="J7" t="s">
-        <v>97</v>
-      </c>
-      <c r="K7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I8" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" t="s">
-        <v>97</v>
-      </c>
-      <c r="K8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>